<commit_message>
Fixed wrong function key assignment in make_tables Updated result tables
</commit_message>
<xml_diff>
--- a/tables/ODE/ODE_table1_dim10.xlsx
+++ b/tables/ODE/ODE_table1_dim10.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40,19 +41,19 @@
     <t>F14</t>
   </si>
   <si>
-    <t>Fc1</t>
-  </si>
-  <si>
-    <t>Fc2</t>
-  </si>
-  <si>
-    <t>Fc6</t>
-  </si>
-  <si>
-    <t>Fc7</t>
-  </si>
-  <si>
-    <t>Fc9</t>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F9</t>
   </si>
 </sst>
 </file>
@@ -69,11 +70,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,15 +101,14 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -401,18 +397,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr>
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">

</xml_diff>